<commit_message>
Figuring out Torch a bit more
</commit_message>
<xml_diff>
--- a/self-driving-car/CarND-Semantic-Segmentation/model_structure.xlsx
+++ b/self-driving-car/CarND-Semantic-Segmentation/model_structure.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\udacity\self-driving-car\CarND-Semantic-Segmentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3375154-A88A-449A-82D1-C47B431E288C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6043C95-09EE-407D-894F-CD1B0C4C7112}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1035" yWindow="1035" windowWidth="23715" windowHeight="14385" xr2:uid="{FE5F3D00-5F79-4D53-9A5C-6C86DBB59148}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="224">
   <si>
     <t>VGG(</t>
   </si>
@@ -171,9 +171,6 @@
     <t xml:space="preserve">    (5): Conv2d(64, 128, kernel_size=(3, 3), stride=(1, 1), padding=(1, 1))</t>
   </si>
   <si>
-    <t>Sequential(</t>
-  </si>
-  <si>
     <t xml:space="preserve">  (0): Conv2d(3, 64, kernel_size=(3, 3), stride=(1, 1), padding=(1, 1))</t>
   </si>
   <si>
@@ -267,36 +264,6 @@
     <t xml:space="preserve">  (30): MaxPool2d(kernel_size=2, stride=2, padding=0, dilation=1, ceil_mode=False)</t>
   </si>
   <si>
-    <t>Conv2d(3, 64, kernel_size=(3, 3), stride=(1, 1), padding=(1, 1))</t>
-  </si>
-  <si>
-    <t>ReLU(inplace=True)</t>
-  </si>
-  <si>
-    <t>Conv2d(64, 64, kernel_size=(3, 3), stride=(1, 1), padding=(1, 1))</t>
-  </si>
-  <si>
-    <t>MaxPool2d(kernel_size=2, stride=2, padding=0, dilation=1, ceil_mode=False)</t>
-  </si>
-  <si>
-    <t>Conv2d(64, 128, kernel_size=(3, 3), stride=(1, 1), padding=(1, 1))</t>
-  </si>
-  <si>
-    <t>Conv2d(128, 128, kernel_size=(3, 3), stride=(1, 1), padding=(1, 1))</t>
-  </si>
-  <si>
-    <t>Conv2d(128, 256, kernel_size=(3, 3), stride=(1, 1), padding=(1, 1))</t>
-  </si>
-  <si>
-    <t>Conv2d(256, 256, kernel_size=(3, 3), stride=(1, 1), padding=(1, 1))</t>
-  </si>
-  <si>
-    <t>Conv2d(256, 512, kernel_size=(3, 3), stride=(1, 1), padding=(1, 1))</t>
-  </si>
-  <si>
-    <t>Conv2d(512, 512, kernel_size=(3, 3), stride=(1, 1), padding=(1, 1))</t>
-  </si>
-  <si>
     <t xml:space="preserve">  (0): Linear(in_features=25088, out_features=4096, bias=True)</t>
   </si>
   <si>
@@ -315,18 +282,6 @@
     <t xml:space="preserve">  (6): Linear(in_features=4096, out_features=1000, bias=True)</t>
   </si>
   <si>
-    <t>Linear(in_features=25088, out_features=4096, bias=True)</t>
-  </si>
-  <si>
-    <t>Dropout(p=0.5, inplace=False)</t>
-  </si>
-  <si>
-    <t>Linear(in_features=4096, out_features=4096, bias=True)</t>
-  </si>
-  <si>
-    <t>Linear(in_features=4096, out_features=1000, bias=True)</t>
-  </si>
-  <si>
     <t>input_1 (InputLayer)         [(None, 224, 224, 3)]     0        'input_1:0' # Walkthrough: so we can pass through image</t>
   </si>
   <si>
@@ -613,6 +568,144 @@
   </si>
   <si>
     <t>Model after adding decoder layers VGG TF2 Keras:</t>
+  </si>
+  <si>
+    <t>module 0 VGG(</t>
+  </si>
+  <si>
+    <t>module 1 Sequential(</t>
+  </si>
+  <si>
+    <t>module 2 Conv2d(3, 64, kernel_size=(3, 3), stride=(1, 1), padding=(1, 1))</t>
+  </si>
+  <si>
+    <t>module 3 ReLU(inplace=True)</t>
+  </si>
+  <si>
+    <t>module 4 Conv2d(64, 64, kernel_size=(3, 3), stride=(1, 1), padding=(1, 1))</t>
+  </si>
+  <si>
+    <t>module 5 ReLU(inplace=True)</t>
+  </si>
+  <si>
+    <t>module 6 MaxPool2d(kernel_size=2, stride=2, padding=0, dilation=1, ceil_mode=False)</t>
+  </si>
+  <si>
+    <t>module 7 Conv2d(64, 128, kernel_size=(3, 3), stride=(1, 1), padding=(1, 1))</t>
+  </si>
+  <si>
+    <t>module 8 ReLU(inplace=True)</t>
+  </si>
+  <si>
+    <t>module 9 Conv2d(128, 128, kernel_size=(3, 3), stride=(1, 1), padding=(1, 1))</t>
+  </si>
+  <si>
+    <t>module 10 ReLU(inplace=True)</t>
+  </si>
+  <si>
+    <t>module 11 MaxPool2d(kernel_size=2, stride=2, padding=0, dilation=1, ceil_mode=False)</t>
+  </si>
+  <si>
+    <t>module 12 Conv2d(128, 256, kernel_size=(3, 3), stride=(1, 1), padding=(1, 1))</t>
+  </si>
+  <si>
+    <t>module 13 ReLU(inplace=True)</t>
+  </si>
+  <si>
+    <t>module 14 Conv2d(256, 256, kernel_size=(3, 3), stride=(1, 1), padding=(1, 1))</t>
+  </si>
+  <si>
+    <t>module 15 ReLU(inplace=True)</t>
+  </si>
+  <si>
+    <t>module 16 Conv2d(256, 256, kernel_size=(3, 3), stride=(1, 1), padding=(1, 1))</t>
+  </si>
+  <si>
+    <t>module 17 ReLU(inplace=True)</t>
+  </si>
+  <si>
+    <t>module 18 MaxPool2d(kernel_size=2, stride=2, padding=0, dilation=1, ceil_mode=False)</t>
+  </si>
+  <si>
+    <t>module 19 Conv2d(256, 512, kernel_size=(3, 3), stride=(1, 1), padding=(1, 1))</t>
+  </si>
+  <si>
+    <t>module 20 ReLU(inplace=True)</t>
+  </si>
+  <si>
+    <t>module 21 Conv2d(512, 512, kernel_size=(3, 3), stride=(1, 1), padding=(1, 1))</t>
+  </si>
+  <si>
+    <t>module 22 ReLU(inplace=True)</t>
+  </si>
+  <si>
+    <t>module 23 Conv2d(512, 512, kernel_size=(3, 3), stride=(1, 1), padding=(1, 1))</t>
+  </si>
+  <si>
+    <t>module 24 ReLU(inplace=True)</t>
+  </si>
+  <si>
+    <t>module 25 MaxPool2d(kernel_size=2, stride=2, padding=0, dilation=1, ceil_mode=False)</t>
+  </si>
+  <si>
+    <t>module 26 Conv2d(512, 512, kernel_size=(3, 3), stride=(1, 1), padding=(1, 1))</t>
+  </si>
+  <si>
+    <t>module 27 ReLU(inplace=True)</t>
+  </si>
+  <si>
+    <t>module 28 Conv2d(512, 512, kernel_size=(3, 3), stride=(1, 1), padding=(1, 1))</t>
+  </si>
+  <si>
+    <t>module 29 ReLU(inplace=True)</t>
+  </si>
+  <si>
+    <t>module 30 Conv2d(512, 512, kernel_size=(3, 3), stride=(1, 1), padding=(1, 1))</t>
+  </si>
+  <si>
+    <t>module 31 ReLU(inplace=True)</t>
+  </si>
+  <si>
+    <t>module 32 MaxPool2d(kernel_size=2, stride=2, padding=0, dilation=1, ceil_mode=False)</t>
+  </si>
+  <si>
+    <t>module 33 AdaptiveAvgPool2d(output_size=(7, 7))</t>
+  </si>
+  <si>
+    <t>module 34 Sequential(</t>
+  </si>
+  <si>
+    <t>module 35 Linear(in_features=25088, out_features=4096, bias=True)</t>
+  </si>
+  <si>
+    <t>module 36 ReLU(inplace=True)</t>
+  </si>
+  <si>
+    <t>module 37 Dropout(p=0.5, inplace=False)</t>
+  </si>
+  <si>
+    <t>module 38 Linear(in_features=4096, out_features=4096, bias=True)</t>
+  </si>
+  <si>
+    <t>module 39 ReLU(inplace=True)</t>
+  </si>
+  <si>
+    <t>module 40 Dropout(p=0.5, inplace=False)</t>
+  </si>
+  <si>
+    <t>module 41 Linear(in_features=4096, out_features=1000, bias=True)</t>
+  </si>
+  <si>
+    <t>Children:</t>
+  </si>
+  <si>
+    <t>child 0 Sequential(</t>
+  </si>
+  <si>
+    <t>child 1 AdaptiveAvgPool2d(output_size=(7, 7))</t>
+  </si>
+  <si>
+    <t>child 2 Sequential(</t>
   </si>
 </sst>
 </file>
@@ -963,10 +1056,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12DDDFEA-BBB8-461C-8062-39C253FCEDDD}">
-  <dimension ref="A1:W200"/>
+  <dimension ref="A1:W246"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J13" workbookViewId="0">
-      <selection activeCell="V50" sqref="V50"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="P49" sqref="P49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -976,26 +1069,26 @@
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="W1" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="W2" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
       <c r="I3" t="s">
-        <v>190</v>
+        <v>175</v>
       </c>
       <c r="O3" t="s">
-        <v>191</v>
+        <v>176</v>
       </c>
       <c r="W3" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.2">
@@ -1008,13 +1101,13 @@
         <v>1</v>
       </c>
       <c r="I5" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
       <c r="O5" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="W5" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.2">
@@ -1022,13 +1115,13 @@
         <v>2</v>
       </c>
       <c r="I6" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="O6" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="W6" t="s">
-        <v>154</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.2">
@@ -1041,13 +1134,13 @@
         <v>4</v>
       </c>
       <c r="I8" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="O8" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="W8" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.2">
@@ -1060,13 +1153,13 @@
         <v>6</v>
       </c>
       <c r="I10" t="s">
-        <v>126</v>
+        <v>111</v>
       </c>
       <c r="O10" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="W10" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.2">
@@ -1074,13 +1167,13 @@
         <v>7</v>
       </c>
       <c r="I11" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
       <c r="O11" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="W11" t="s">
-        <v>157</v>
+        <v>142</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.2">
@@ -1093,13 +1186,13 @@
         <v>9</v>
       </c>
       <c r="I13" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
       <c r="O13" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="W13" t="s">
-        <v>158</v>
+        <v>143</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.2">
@@ -1112,13 +1205,13 @@
         <v>11</v>
       </c>
       <c r="I15" t="s">
-        <v>129</v>
+        <v>114</v>
       </c>
       <c r="O15" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="W15" t="s">
-        <v>159</v>
+        <v>144</v>
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.2">
@@ -1126,13 +1219,13 @@
         <v>12</v>
       </c>
       <c r="I16" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="O16" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="W16" t="s">
-        <v>160</v>
+        <v>145</v>
       </c>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.2">
@@ -1145,13 +1238,13 @@
         <v>14</v>
       </c>
       <c r="I18" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="O18" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="W18" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.2">
@@ -1164,13 +1257,13 @@
         <v>16</v>
       </c>
       <c r="I20" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
       <c r="O20" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="W20" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.2">
@@ -1183,13 +1276,13 @@
         <v>18</v>
       </c>
       <c r="I22" t="s">
-        <v>133</v>
+        <v>118</v>
       </c>
       <c r="O22" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="W22" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.2">
@@ -1197,13 +1290,13 @@
         <v>19</v>
       </c>
       <c r="I23" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="O23" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
       <c r="W23" t="s">
-        <v>164</v>
+        <v>149</v>
       </c>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.2">
@@ -1216,13 +1309,13 @@
         <v>21</v>
       </c>
       <c r="I25" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="O25" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="W25" t="s">
-        <v>165</v>
+        <v>150</v>
       </c>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.2">
@@ -1235,13 +1328,13 @@
         <v>23</v>
       </c>
       <c r="I27" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="O27" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="W27" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.2">
@@ -1254,13 +1347,13 @@
         <v>25</v>
       </c>
       <c r="I29" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
       <c r="O29" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
       <c r="W29" t="s">
-        <v>167</v>
+        <v>152</v>
       </c>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.2">
@@ -1268,13 +1361,13 @@
         <v>26</v>
       </c>
       <c r="I30" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
       <c r="O30" t="s">
-        <v>112</v>
+        <v>97</v>
       </c>
       <c r="W30" t="s">
-        <v>168</v>
+        <v>153</v>
       </c>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.2">
@@ -1287,13 +1380,13 @@
         <v>28</v>
       </c>
       <c r="I32" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="O32" t="s">
-        <v>113</v>
+        <v>98</v>
       </c>
       <c r="W32" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.2">
@@ -1306,13 +1399,13 @@
         <v>30</v>
       </c>
       <c r="I34" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="O34" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="W34" t="s">
-        <v>170</v>
+        <v>155</v>
       </c>
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.2">
@@ -1325,16 +1418,16 @@
         <v>32</v>
       </c>
       <c r="I36" t="s">
-        <v>141</v>
+        <v>126</v>
       </c>
       <c r="O36" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="V36" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="W36" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
     </row>
     <row r="37" spans="1:23" x14ac:dyDescent="0.2">
@@ -1347,10 +1440,10 @@
         <v>34</v>
       </c>
       <c r="O38" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="T38" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
     </row>
     <row r="39" spans="1:23" x14ac:dyDescent="0.2">
@@ -1358,7 +1451,7 @@
         <v>35</v>
       </c>
       <c r="V39" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
     </row>
     <row r="40" spans="1:23" x14ac:dyDescent="0.2">
@@ -1366,10 +1459,10 @@
         <v>36</v>
       </c>
       <c r="I40" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="O40" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
     </row>
     <row r="41" spans="1:23" x14ac:dyDescent="0.2">
@@ -1382,10 +1475,10 @@
         <v>37</v>
       </c>
       <c r="I42" t="s">
-        <v>143</v>
+        <v>128</v>
       </c>
       <c r="O42" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
     </row>
     <row r="43" spans="1:23" x14ac:dyDescent="0.2">
@@ -1393,10 +1486,10 @@
         <v>38</v>
       </c>
       <c r="I43" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="O43" t="s">
-        <v>118</v>
+        <v>103</v>
       </c>
     </row>
     <row r="44" spans="1:23" x14ac:dyDescent="0.2">
@@ -1409,10 +1502,10 @@
         <v>40</v>
       </c>
       <c r="I45" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
       <c r="O45" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
     </row>
     <row r="46" spans="1:23" x14ac:dyDescent="0.2">
@@ -1420,10 +1513,10 @@
         <v>41</v>
       </c>
       <c r="I46" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
       <c r="O46" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
     </row>
     <row r="47" spans="1:23" x14ac:dyDescent="0.2">
@@ -1436,85 +1529,85 @@
         <v>42</v>
       </c>
       <c r="I48" t="s">
-        <v>183</v>
+        <v>168</v>
       </c>
       <c r="W48" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
     </row>
     <row r="50" spans="9:23" x14ac:dyDescent="0.2">
       <c r="I50" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="W50" t="s">
-        <v>173</v>
+        <v>158</v>
       </c>
     </row>
     <row r="51" spans="9:23" x14ac:dyDescent="0.2">
       <c r="I51" t="s">
-        <v>185</v>
+        <v>170</v>
       </c>
       <c r="W51" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
     </row>
     <row r="53" spans="9:23" x14ac:dyDescent="0.2">
       <c r="I53" t="s">
-        <v>186</v>
+        <v>171</v>
       </c>
       <c r="W53" t="s">
-        <v>175</v>
+        <v>160</v>
       </c>
     </row>
     <row r="55" spans="9:23" x14ac:dyDescent="0.2">
       <c r="I55" t="s">
-        <v>187</v>
+        <v>172</v>
       </c>
       <c r="W55" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
     </row>
     <row r="57" spans="9:23" x14ac:dyDescent="0.2">
       <c r="I57" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
       <c r="W57" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
     </row>
     <row r="58" spans="9:23" x14ac:dyDescent="0.2">
       <c r="W58" t="s">
-        <v>178</v>
+        <v>163</v>
       </c>
     </row>
     <row r="59" spans="9:23" x14ac:dyDescent="0.2">
       <c r="I59" t="s">
-        <v>189</v>
+        <v>174</v>
       </c>
     </row>
     <row r="60" spans="9:23" x14ac:dyDescent="0.2">
       <c r="W60" t="s">
-        <v>179</v>
+        <v>164</v>
       </c>
     </row>
     <row r="61" spans="9:23" x14ac:dyDescent="0.2">
       <c r="W61" t="s">
-        <v>152</v>
+        <v>137</v>
       </c>
     </row>
     <row r="62" spans="9:23" x14ac:dyDescent="0.2">
       <c r="W62" t="s">
-        <v>180</v>
+        <v>165</v>
       </c>
     </row>
     <row r="63" spans="9:23" x14ac:dyDescent="0.2">
       <c r="W63" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
     </row>
     <row r="64" spans="9:23" x14ac:dyDescent="0.2">
       <c r="W64" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
@@ -1524,7 +1617,7 @@
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>0</v>
+        <v>178</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
@@ -1749,162 +1842,162 @@
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>45</v>
+        <v>179</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.2">
@@ -1914,237 +2007,462 @@
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>77</v>
+        <v>180</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>78</v>
+        <v>181</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>79</v>
+        <v>182</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>78</v>
+        <v>183</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>80</v>
+        <v>184</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>81</v>
+        <v>185</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>78</v>
+        <v>186</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>82</v>
+        <v>187</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>78</v>
+        <v>188</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>80</v>
+        <v>189</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>83</v>
+        <v>190</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>78</v>
+        <v>191</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>84</v>
+        <v>192</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>78</v>
+        <v>193</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>84</v>
+        <v>194</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>78</v>
+        <v>195</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>80</v>
+        <v>196</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>85</v>
+        <v>197</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>78</v>
+        <v>198</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>86</v>
+        <v>199</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>78</v>
+        <v>200</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>86</v>
+        <v>201</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>78</v>
+        <v>202</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>80</v>
+        <v>203</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>86</v>
+        <v>204</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>78</v>
+        <v>205</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>86</v>
+        <v>206</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>78</v>
+        <v>207</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>86</v>
+        <v>208</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>78</v>
+        <v>209</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>80</v>
+        <v>210</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>45</v>
+        <v>211</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>87</v>
+        <v>212</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>47</v>
+        <v>76</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>88</v>
+        <v>46</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>42</v>
+        <v>81</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>93</v>
+        <v>42</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>78</v>
+        <v>213</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>94</v>
+        <v>214</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>95</v>
+        <v>215</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>78</v>
+        <v>216</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>94</v>
+        <v>217</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>96</v>
+        <v>218</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A201" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A203" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A204" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A205" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A206" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A207" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A208" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A209" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A210" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A211" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A212" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A213" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A214" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A215" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A216" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A217" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A218" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="219" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A219" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A220" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="221" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A221" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A222" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="223" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A223" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A224" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A225" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A226" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="227" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A227" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A228" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="229" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A229" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A230" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="231" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A231" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A232" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="233" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A233" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A234" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="235" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A235" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="236" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A236" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="237" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A237" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="238" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A238" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="239" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A239" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="240" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A240" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="241" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A241" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="242" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A242" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="243" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A243" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="244" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A244" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="245" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A245" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="246" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A246" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sketched out more PyTorch implementation, almost certainly wrongly at this point
</commit_message>
<xml_diff>
--- a/self-driving-car/CarND-Semantic-Segmentation/model_structure.xlsx
+++ b/self-driving-car/CarND-Semantic-Segmentation/model_structure.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\udacity\self-driving-car\CarND-Semantic-Segmentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6043C95-09EE-407D-894F-CD1B0C4C7112}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD9A90FA-C8FB-436D-BD74-717482B28E20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1035" yWindow="1035" windowWidth="23715" windowHeight="14385" xr2:uid="{FE5F3D00-5F79-4D53-9A5C-6C86DBB59148}"/>
   </bookViews>
@@ -336,9 +336,6 @@
     <t>block5_conv3 (Conv2D)        (None, 14, 14, 512)       2359808</t>
   </si>
   <si>
-    <t>block5_pool (MaxPooling2D)   (None, 7, 7, 512)         0          'layer7_out:0'  # Walkthrough: pool5 layer</t>
-  </si>
-  <si>
     <t>flatten (Flatten)            (None, 25088)             0</t>
   </si>
   <si>
@@ -706,6 +703,9 @@
   </si>
   <si>
     <t>child 2 Sequential(</t>
+  </si>
+  <si>
+    <t>block5_pool (MaxPooling2D)   (None, 7, 7, 512)         0          'layer7[no that was bug!]_out:0'  # Walkthrough: pool5 layer</t>
   </si>
 </sst>
 </file>
@@ -1058,8 +1058,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12DDDFEA-BBB8-461C-8062-39C253FCEDDD}">
   <dimension ref="A1:W246"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="P49" sqref="P49"/>
+    <sheetView tabSelected="1" topLeftCell="J26" workbookViewId="0">
+      <selection activeCell="O50" sqref="O50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1069,26 +1069,26 @@
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="W1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="W2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I3" t="s">
+        <v>174</v>
+      </c>
+      <c r="O3" t="s">
         <v>175</v>
       </c>
-      <c r="O3" t="s">
-        <v>176</v>
-      </c>
       <c r="W3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.2">
@@ -1101,13 +1101,13 @@
         <v>1</v>
       </c>
       <c r="I5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="O5" t="s">
         <v>82</v>
       </c>
       <c r="W5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.2">
@@ -1115,13 +1115,13 @@
         <v>2</v>
       </c>
       <c r="I6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="O6" t="s">
         <v>83</v>
       </c>
       <c r="W6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.2">
@@ -1134,13 +1134,13 @@
         <v>4</v>
       </c>
       <c r="I8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="O8" t="s">
         <v>84</v>
       </c>
       <c r="W8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.2">
@@ -1153,13 +1153,13 @@
         <v>6</v>
       </c>
       <c r="I10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="O10" t="s">
         <v>85</v>
       </c>
       <c r="W10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.2">
@@ -1167,13 +1167,13 @@
         <v>7</v>
       </c>
       <c r="I11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="O11" t="s">
         <v>86</v>
       </c>
       <c r="W11" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.2">
@@ -1186,13 +1186,13 @@
         <v>9</v>
       </c>
       <c r="I13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="O13" t="s">
         <v>87</v>
       </c>
       <c r="W13" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.2">
@@ -1205,13 +1205,13 @@
         <v>11</v>
       </c>
       <c r="I15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="O15" t="s">
         <v>88</v>
       </c>
       <c r="W15" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.2">
@@ -1219,13 +1219,13 @@
         <v>12</v>
       </c>
       <c r="I16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="O16" t="s">
         <v>89</v>
       </c>
       <c r="W16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.2">
@@ -1238,13 +1238,13 @@
         <v>14</v>
       </c>
       <c r="I18" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="O18" t="s">
         <v>90</v>
       </c>
       <c r="W18" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.2">
@@ -1257,13 +1257,13 @@
         <v>16</v>
       </c>
       <c r="I20" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="O20" t="s">
         <v>91</v>
       </c>
       <c r="W20" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.2">
@@ -1276,13 +1276,13 @@
         <v>18</v>
       </c>
       <c r="I22" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="O22" t="s">
         <v>92</v>
       </c>
       <c r="W22" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.2">
@@ -1290,13 +1290,13 @@
         <v>19</v>
       </c>
       <c r="I23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="O23" t="s">
         <v>93</v>
       </c>
       <c r="W23" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.2">
@@ -1309,13 +1309,13 @@
         <v>21</v>
       </c>
       <c r="I25" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="O25" t="s">
         <v>94</v>
       </c>
       <c r="W25" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.2">
@@ -1328,13 +1328,13 @@
         <v>23</v>
       </c>
       <c r="I27" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="O27" t="s">
         <v>95</v>
       </c>
       <c r="W27" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.2">
@@ -1347,13 +1347,13 @@
         <v>25</v>
       </c>
       <c r="I29" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="O29" t="s">
         <v>96</v>
       </c>
       <c r="W29" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.2">
@@ -1361,13 +1361,13 @@
         <v>26</v>
       </c>
       <c r="I30" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="O30" t="s">
         <v>97</v>
       </c>
       <c r="W30" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.2">
@@ -1380,13 +1380,13 @@
         <v>28</v>
       </c>
       <c r="I32" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="O32" t="s">
         <v>98</v>
       </c>
       <c r="W32" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.2">
@@ -1399,13 +1399,13 @@
         <v>30</v>
       </c>
       <c r="I34" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="O34" t="s">
         <v>99</v>
       </c>
       <c r="W34" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.2">
@@ -1418,16 +1418,16 @@
         <v>32</v>
       </c>
       <c r="I36" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="O36" t="s">
-        <v>100</v>
+        <v>223</v>
       </c>
       <c r="V36" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="W36" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="37" spans="1:23" x14ac:dyDescent="0.2">
@@ -1440,10 +1440,10 @@
         <v>34</v>
       </c>
       <c r="O38" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="T38" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="39" spans="1:23" x14ac:dyDescent="0.2">
@@ -1451,7 +1451,7 @@
         <v>35</v>
       </c>
       <c r="V39" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="40" spans="1:23" x14ac:dyDescent="0.2">
@@ -1459,10 +1459,10 @@
         <v>36</v>
       </c>
       <c r="I40" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="O40" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="41" spans="1:23" x14ac:dyDescent="0.2">
@@ -1475,10 +1475,10 @@
         <v>37</v>
       </c>
       <c r="I42" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O42" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="43" spans="1:23" x14ac:dyDescent="0.2">
@@ -1486,10 +1486,10 @@
         <v>38</v>
       </c>
       <c r="I43" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="O43" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="44" spans="1:23" x14ac:dyDescent="0.2">
@@ -1502,10 +1502,10 @@
         <v>40</v>
       </c>
       <c r="I45" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="O45" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="46" spans="1:23" x14ac:dyDescent="0.2">
@@ -1513,10 +1513,10 @@
         <v>41</v>
       </c>
       <c r="I46" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="O46" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="47" spans="1:23" x14ac:dyDescent="0.2">
@@ -1529,85 +1529,85 @@
         <v>42</v>
       </c>
       <c r="I48" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="W48" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="50" spans="9:23" x14ac:dyDescent="0.2">
       <c r="I50" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="W50" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="51" spans="9:23" x14ac:dyDescent="0.2">
       <c r="I51" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="W51" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="53" spans="9:23" x14ac:dyDescent="0.2">
       <c r="I53" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="W53" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="55" spans="9:23" x14ac:dyDescent="0.2">
       <c r="I55" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="W55" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="57" spans="9:23" x14ac:dyDescent="0.2">
       <c r="I57" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="W57" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="58" spans="9:23" x14ac:dyDescent="0.2">
       <c r="W58" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="59" spans="9:23" x14ac:dyDescent="0.2">
       <c r="I59" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="60" spans="9:23" x14ac:dyDescent="0.2">
       <c r="W60" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="61" spans="9:23" x14ac:dyDescent="0.2">
       <c r="W61" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="62" spans="9:23" x14ac:dyDescent="0.2">
       <c r="W62" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="63" spans="9:23" x14ac:dyDescent="0.2">
       <c r="W63" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="64" spans="9:23" x14ac:dyDescent="0.2">
       <c r="W64" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
@@ -1617,7 +1617,7 @@
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
@@ -1842,7 +1842,7 @@
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.2">
@@ -2007,167 +2007,167 @@
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.2">
@@ -2212,47 +2212,47 @@
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.2">
@@ -2417,12 +2417,12 @@
     </row>
     <row r="237" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="238" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="239" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>